<commit_message>
Updated tutorial with Aislyn's comments
</commit_message>
<xml_diff>
--- a/Tutorial/EncountersDoubleTutorial.xlsx
+++ b/Tutorial/EncountersDoubleTutorial.xlsx
@@ -153,7 +153,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -185,7 +185,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>1</v>
@@ -199,10 +199,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>2</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -213,10 +213,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>